<commit_message>
all data from It collected
</commit_message>
<xml_diff>
--- a/2-the-martian/the-martian.xlsx
+++ b/2-the-martian/the-martian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/2-the-martian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{85DB4856-6364-5D4D-A9B2-9C0EC7A6416C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{26B890FE-BCAE-1C42-8F5D-9AC3B5797B28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25180" yWindow="4200" windowWidth="24040" windowHeight="22780" xr2:uid="{9B493D7A-610D-0D44-8370-5F1EB02042AC}"/>
   </bookViews>
@@ -50,12 +50,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,13 +99,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,52 +1502,52 @@
         <v>42427</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
+    <row r="72" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
         <v>42449</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="5">
         <v>5</v>
       </c>
-      <c r="C72" s="2">
-        <v>15</v>
-      </c>
-      <c r="D72" s="3">
+      <c r="C72" s="5">
+        <v>15</v>
+      </c>
+      <c r="D72" s="4">
         <f t="shared" si="1"/>
         <v>42434</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
+    </row>
+    <row r="73" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
         <v>42456</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="5">
         <v>6</v>
       </c>
-      <c r="C73">
-        <v>15</v>
-      </c>
-      <c r="D73" s="1">
+      <c r="C73" s="5">
+        <v>15</v>
+      </c>
+      <c r="D73" s="4">
         <f t="shared" si="1"/>
         <v>42441</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
+    <row r="74" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="7">
         <v>42463</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="6">
         <v>5</v>
       </c>
-      <c r="C74">
-        <v>15</v>
-      </c>
-      <c r="D74" s="1">
+      <c r="C74" s="6">
+        <v>15</v>
+      </c>
+      <c r="D74" s="7">
         <f t="shared" si="1"/>
         <v>42448</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>